<commit_message>
perfect ladder simulation complete
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15440"/>
+    <workbookView windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>name</t>
   </si>
@@ -47,57 +47,6 @@
   </si>
   <si>
     <t>G</t>
-  </si>
-  <si>
-    <t>(Am)</t>
-  </si>
-  <si>
-    <t>(Um)</t>
-  </si>
-  <si>
-    <t>Cm</t>
-  </si>
-  <si>
-    <t>(CU)</t>
-  </si>
-  <si>
-    <t>(CA)</t>
-  </si>
-  <si>
-    <t>(CG)</t>
-  </si>
-  <si>
-    <t>(UA)</t>
-  </si>
-  <si>
-    <t>(UG)</t>
-  </si>
-  <si>
-    <t>(AG)</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>mG</t>
-  </si>
-  <si>
-    <t>acp3U</t>
-  </si>
-  <si>
-    <t>C'</t>
-  </si>
-  <si>
-    <t>(CC)</t>
-  </si>
-  <si>
-    <t>(UU)</t>
-  </si>
-  <si>
-    <t>(AA)</t>
-  </si>
-  <si>
-    <t>(GG)</t>
   </si>
 </sst>
 </file>
@@ -1028,13 +977,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
     <col min="2" max="2" width="11.625"/>
     <col min="4" max="4" width="10.5"/>
@@ -1081,206 +1030,6 @@
         <v>345.0474</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>343.06817</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>320.04095</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>319.05694</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <f>B4+B5</f>
-        <v>674.0999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <f>B2+B4</f>
-        <v>634.0938</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <f>B2+B5</f>
-        <v>650.0887</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <f>B3+B4</f>
-        <v>635.0778</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13">
-        <f>B3+B5</f>
-        <v>651.0727</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <f>B4+B5</f>
-        <v>674.0999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>308.0412</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16">
-        <v>359.0612</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>407.0834</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>307.03</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <f>B2*2</f>
-        <v>610.0826</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20">
-        <f>B3*2</f>
-        <v>612.0506</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <f>B4*2</f>
-        <v>658.105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22">
-        <f>B5*2</f>
-        <v>690.0948</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23">
-        <f>B2+B3</f>
-        <v>611.0666</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24">
-        <f>B2+B4</f>
-        <v>634.0938</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25">
-        <f>B2+B5</f>
-        <v>650.0887</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26">
-        <f>B3+B4</f>
-        <v>635.0778</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27">
-        <f>B3+B5</f>
-        <v>651.0727</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28">
-        <f>B4+B5</f>
-        <v>674.0999</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>